<commit_message>
Update: PDF coordinates updated.
</commit_message>
<xml_diff>
--- a/userdata-backups/2.xlsx
+++ b/userdata-backups/2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="608">
   <si>
     <t>Name</t>
   </si>
@@ -2247,7 +2247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="1">"Frederick J. Boyd (" &amp; F3 &amp; ")"</f>
         <v>Frederick J. Boyd (0002)</v>
@@ -2272,8 +2272,11 @@
         <f t="shared" si="0"/>
         <v>0002</v>
       </c>
-    </row>
-    <row r="4" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0003)</v>
@@ -2298,8 +2301,11 @@
         <f t="shared" si="0"/>
         <v>0003</v>
       </c>
-    </row>
-    <row r="5" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0004)</v>
@@ -2324,8 +2330,11 @@
         <f t="shared" si="0"/>
         <v>0004</v>
       </c>
-    </row>
-    <row r="6" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0005)</v>
@@ -2350,8 +2359,11 @@
         <f t="shared" si="0"/>
         <v>0005</v>
       </c>
-    </row>
-    <row r="7" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0006)</v>
@@ -2376,8 +2388,11 @@
         <f t="shared" si="0"/>
         <v>0006</v>
       </c>
-    </row>
-    <row r="8" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0007)</v>
@@ -2402,8 +2417,11 @@
         <f t="shared" si="0"/>
         <v>0007</v>
       </c>
-    </row>
-    <row r="9" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0008)</v>
@@ -2428,8 +2446,11 @@
         <f t="shared" si="0"/>
         <v>0008</v>
       </c>
-    </row>
-    <row r="10" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0009)</v>
@@ -2454,8 +2475,11 @@
         <f t="shared" si="0"/>
         <v>0009</v>
       </c>
-    </row>
-    <row r="11" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0010)</v>
@@ -2480,8 +2504,11 @@
         <f t="shared" si="0"/>
         <v>0010</v>
       </c>
-    </row>
-    <row r="12" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0011)</v>
@@ -2506,8 +2533,11 @@
         <f t="shared" si="0"/>
         <v>0011</v>
       </c>
-    </row>
-    <row r="13" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0012)</v>
@@ -2532,8 +2562,11 @@
         <f t="shared" si="0"/>
         <v>0012</v>
       </c>
-    </row>
-    <row r="14" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0013)</v>
@@ -2557,6 +2590,9 @@
       <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>0013</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2585,7 +2621,7 @@
         <v>0014</v>
       </c>
     </row>
-    <row r="16" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" ht="16" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="1"/>
         <v>Frederick J. Boyd (0015)</v>
@@ -2609,6 +2645,9 @@
       <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>0015</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" ht="16" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>